<commit_message>
Formatted testing document so that there is a seperate sheet for each gui window being test. Each test case has a description, sequence of inputs/actions for the user to take, the expected output, the output from the test, a cell to indicate whether the test passed or failed, and the date in which the test was conducted.
</commit_message>
<xml_diff>
--- a/src/test/manualtests/ManualTesting.xlsx
+++ b/src/test/manualtests/ManualTesting.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quinn\IdeaProjects\team-15\src\test\manualtests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC6A3BA5-F2CA-4707-B856-819950D2D94F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A0101CF-70B6-4A72-BC3E-DEBA0B17E0F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{75FEE4CB-4BE4-41F5-B058-761CC4F28A61}"/>
+    <workbookView xWindow="-19280" yWindow="-80" windowWidth="19360" windowHeight="10360" xr2:uid="{75FEE4CB-4BE4-41F5-B058-761CC4F28A61}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="MenuWindow" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,9 +35,49 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>Test Description</t>
+  </si>
+  <si>
+    <t>Sequence of Inputs</t>
+  </si>
+  <si>
+    <t>Test Output</t>
+  </si>
+  <si>
+    <t>Expected Output</t>
+  </si>
+  <si>
+    <t>Pass/Fail</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Menu Window</t>
+  </si>
+  <si>
+    <t>Error message pops up with 3 messages on what the player needs to do to play the game. Those being to enter a valid name, select a difficulty, and select 3 towers.</t>
+  </si>
+  <si>
+    <t>The error dialog pops up with all 3 messages.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Leave the name input blank
+ - Leave the difficulty and towers unselected
+ - Click play button </t>
+  </si>
+  <si>
+    <t>Testing the error detection when nothing is selected</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -45,16 +85,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -62,12 +123,104 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,12 +555,275 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A5FDB90-F59B-42F0-ACD5-CFB18DAB7460}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="131" zoomScaleNormal="131" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="33.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="29.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="9">
+        <v>45433</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>